<commit_message>
generated algorithm to generate spend transactions
</commit_message>
<xml_diff>
--- a/david_finance.xlsx
+++ b/david_finance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\python_codes\david_finance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\python_codes\finance_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AC24F1-A99B-4064-82E1-DB1F24B9B62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B5DBCD-F0EE-4234-822D-42CB6D8BE55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{345403B4-E0C2-451B-BA1E-8F2416887F82}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{345403B4-E0C2-451B-BA1E-8F2416887F82}"/>
   </bookViews>
   <sheets>
     <sheet name="nueva_deuda_a_plazos" sheetId="2" r:id="rId1"/>
@@ -23,19 +23,21 @@
     <sheet name="ingresos_categories" sheetId="17" r:id="rId8"/>
     <sheet name="issued_by" sheetId="12" r:id="rId9"/>
     <sheet name="tarjetas_de_credito" sheetId="13" r:id="rId10"/>
-    <sheet name="creditos" sheetId="18" r:id="rId11"/>
-    <sheet name="debito_y_cuentas" sheetId="14" r:id="rId12"/>
-    <sheet name="frecuencias_de_pago" sheetId="15" r:id="rId13"/>
-    <sheet name="plazos_recurrente_normal" sheetId="16" r:id="rId14"/>
+    <sheet name="payment_methods" sheetId="19" r:id="rId11"/>
+    <sheet name="creditos" sheetId="18" r:id="rId12"/>
+    <sheet name="debito_y_cuentas" sheetId="14" r:id="rId13"/>
+    <sheet name="frecuencias_de_pago" sheetId="15" r:id="rId14"/>
+    <sheet name="plazos_recurrente_normal" sheetId="16" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="creditos">tbl_creditos[[#All],[creditos]]</definedName>
+    <definedName name="credit_cards">tarjetas_de_credito!$A$2:$A$6</definedName>
+    <definedName name="creditos">creditos!$A$2:$A$7</definedName>
     <definedName name="debito_y_cuentas">debito_y_cuentas!$A$2:$A$6</definedName>
-    <definedName name="frecuencias_de_pago">frecuencias_de_pago!$A$2:$A$9</definedName>
+    <definedName name="frecuencias_de_pago">frecuencias_de_pago!$A$2:$A$10</definedName>
     <definedName name="gastos_categories">gastos_categories!$A$2:$A$32</definedName>
     <definedName name="ingresos_categories">ingresos_categories!$A$2:$A$4</definedName>
     <definedName name="issued_by">issued_by!$A$2:$A$8</definedName>
-    <definedName name="payment_method">tarjetas_de_credito!$A$2:$A$6</definedName>
+    <definedName name="payment_methods">payment_methods!$A$2:$A$11</definedName>
     <definedName name="plazos_recurrente_normal">plazos_recurrente_normal!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="110">
   <si>
     <t>fecha_de_transaccion</t>
   </si>
@@ -148,9 +150,6 @@
     <t>fecha_de_cargo</t>
   </si>
   <si>
-    <t>limite_de_pago</t>
-  </si>
-  <si>
     <t>deuda_a_plazos_recurrente_o_normal</t>
   </si>
   <si>
@@ -253,9 +252,6 @@
     <t>Vaquita</t>
   </si>
   <si>
-    <t>payment_method</t>
-  </si>
-  <si>
     <t>LikeU</t>
   </si>
   <si>
@@ -307,9 +303,6 @@
     <t>dia_de_corte</t>
   </si>
   <si>
-    <t>dia_de_pago</t>
-  </si>
-  <si>
     <t>debito_y_cuentas</t>
   </si>
   <si>
@@ -370,37 +363,34 @@
     <t>Intereses</t>
   </si>
   <si>
-    <t>Comentario de gym</t>
-  </si>
-  <si>
-    <t>Comentario de Impuestos</t>
-  </si>
-  <si>
-    <t>Descripcion de gim</t>
-  </si>
-  <si>
-    <t>Description impuestos</t>
-  </si>
-  <si>
-    <t>Credito nomina afirme</t>
-  </si>
-  <si>
-    <t>Comentario nomina</t>
-  </si>
-  <si>
-    <t>Recibo Gas</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>Registro por deuda de wendy</t>
-  </si>
-  <si>
     <t>creditos</t>
   </si>
   <si>
     <t>plazo_para_pagar</t>
+  </si>
+  <si>
+    <t>trimestral</t>
+  </si>
+  <si>
+    <t>credit_cards</t>
+  </si>
+  <si>
+    <t>payment_methods</t>
+  </si>
+  <si>
+    <t>Reinscripcion</t>
+  </si>
+  <si>
+    <t>Colegiatura</t>
+  </si>
+  <si>
+    <t>Flores Mamá</t>
+  </si>
+  <si>
+    <t>Dia de madres</t>
+  </si>
+  <si>
+    <t>Celular Samsung A54</t>
   </si>
 </sst>
 </file>
@@ -436,15 +426,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="43">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -534,6 +525,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -585,31 +579,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}" name="estructura_transacciones" displayName="estructura_transacciones" ref="A1:K8" totalsRowShown="0">
-  <autoFilter ref="A1:K8" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}" name="estructura_transacciones" displayName="estructura_transacciones" ref="A1:K2" totalsRowShown="0">
+  <autoFilter ref="A1:K2" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3751A530-512A-48D0-ACA1-E2237E85BD4B}" name="fecha_de_transaccion" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{7385DBD7-EB34-433E-A7DB-728EAF33D62E}" name="frecuencia_de_pago" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{626C2B8F-5C27-4C0B-B719-5B93327D2501}" name="fecha_de_inicio" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{3751A530-512A-48D0-ACA1-E2237E85BD4B}" name="fecha_de_transaccion" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{7385DBD7-EB34-433E-A7DB-728EAF33D62E}" name="frecuencia_de_pago" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{626C2B8F-5C27-4C0B-B719-5B93327D2501}" name="fecha_de_inicio" dataDxfId="40"/>
     <tableColumn id="4" xr3:uid="{6FA13EEF-3757-406D-AB04-AE84D502C26F}" name="numero_de_plazos"/>
     <tableColumn id="5" xr3:uid="{69EFA34A-90CC-44D8-94DA-C15E94B31796}" name="dias_de_margen"/>
-    <tableColumn id="6" xr3:uid="{6FA1131D-FE42-43C8-9D6A-591D0F28EC2F}" name="monto_total_deuda" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{FD79B06C-466E-4B3B-92B7-9CC99AB235E6}" name="forma_de_pago" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{3B2495AD-A8F6-48EB-BEEF-5C6D9FDC70A4}" name="descripcion" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{6A11E9C5-3541-40DF-A991-FB22ABA03550}" name="categoria" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{E0E77362-FF5F-42CB-91DD-D5389F8891C5}" name="realizado_por" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{E46B6D76-C8A7-4B91-8651-7A3D1A573011}" name="comentarios" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{6FA1131D-FE42-43C8-9D6A-591D0F28EC2F}" name="monto_total_deuda" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{FD79B06C-466E-4B3B-92B7-9CC99AB235E6}" name="forma_de_pago" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{3B2495AD-A8F6-48EB-BEEF-5C6D9FDC70A4}" name="descripcion" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{6A11E9C5-3541-40DF-A991-FB22ABA03550}" name="categoria" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{E0E77362-FF5F-42CB-91DD-D5389F8891C5}" name="realizado_por" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{E46B6D76-C8A7-4B91-8651-7A3D1A573011}" name="comentarios" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9CFA1823-AEE8-4F63-833F-B72781BDAA8D}" name="tbl_tarjetas_de_credito" displayName="tbl_tarjetas_de_credito" ref="A1:D6" totalsRowShown="0">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{61208F26-2C92-45CC-B249-AC17EA349613}" name="payment_method"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9CFA1823-AEE8-4F63-833F-B72781BDAA8D}" name="tbl_credit_cards" displayName="tbl_credit_cards" ref="A1:C6" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{61208F26-2C92-45CC-B249-AC17EA349613}" name="credit_cards"/>
     <tableColumn id="2" xr3:uid="{6C7D9BEB-9819-4AF2-9F21-D2E6EC717C7C}" name="dia_de_corte"/>
-    <tableColumn id="3" xr3:uid="{9D57C55B-33D7-4B71-8504-ADCCBA0F0B9A}" name="dia_de_pago"/>
     <tableColumn id="4" xr3:uid="{5DFABE5D-C83E-4137-BD37-F42B51A174E8}" name="plazo_para_pagar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -617,6 +610,15 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FB2F1B61-6BB5-4631-AA80-6C4EAC37AA8F}" name="tbl_payment_methods" displayName="tbl_payment_methods" ref="A1:A11" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{3259DA84-A256-4980-9405-0F87438BFD13}" name="payment_methods"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{504B537A-CF9A-4C93-901E-81100B737829}" name="tbl_creditos" displayName="tbl_creditos" ref="A1:A7" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{85F827C8-280F-40ED-8DE7-C1BB7D914AEC}" name="creditos"/>
@@ -625,7 +627,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{965C8E30-D6E9-4403-BA1D-12E9BDF19FCC}" name="tbl_debito_y_cuentas" displayName="tbl_debito_y_cuentas" ref="A1:A6" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{8CAFC42E-D052-4CFF-BB2B-49BA75141D1E}" name="debito_y_cuentas"/>
@@ -634,9 +636,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6A767FC8-F4DE-40D7-AD0A-601AD036E4B9}" name="tbl_frecuencias_de_pago" displayName="tbl_frecuencias_de_pago" ref="A1:A9" totalsRowShown="0">
-  <autoFilter ref="A1:A9" xr:uid="{007A344A-CC5B-4E08-93AD-7E8015A5037B}"/>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6A767FC8-F4DE-40D7-AD0A-601AD036E4B9}" name="tbl_frecuencias_de_pago" displayName="tbl_frecuencias_de_pago" ref="A1:A10" totalsRowShown="0">
+  <autoFilter ref="A1:A10" xr:uid="{007A344A-CC5B-4E08-93AD-7E8015A5037B}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{FA46264A-D1C9-4322-8D7D-69F74DDF7914}" name="frecuencias_de_pago"/>
   </tableColumns>
@@ -644,7 +646,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{E80950E7-1E5E-4DFB-AD5B-05525A9603B0}" name="tbl_plazos_recurrente_normal" displayName="tbl_plazos_recurrente_normal" ref="A1:A4" totalsRowShown="0">
   <autoFilter ref="A1:A4" xr:uid="{E80950E7-1E5E-4DFB-AD5B-05525A9603B0}"/>
   <tableColumns count="1">
@@ -655,15 +657,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F622556F-D87B-4F08-9DB0-55027FD6196C}" name="estructura_transacciones3" displayName="estructura_transacciones3" ref="A1:K3" totalsRowShown="0">
-  <autoFilter ref="A1:K3" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F622556F-D87B-4F08-9DB0-55027FD6196C}" name="estructura_transacciones3" displayName="estructura_transacciones3" ref="A1:K4" totalsRowShown="0">
+  <autoFilter ref="A1:K4" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{596EC6A4-11EF-4DEE-B34E-9EC3BA15F511}" name="fecha_de_transaccion" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{0BAC5350-6187-4007-A1E7-9BB5CEF1C730}" name="frecuencia_de_pago" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{D476E092-13AF-42EE-AEEF-4CD702AD1094}" name="fecha_de_inicio" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{596EC6A4-11EF-4DEE-B34E-9EC3BA15F511}" name="fecha_de_transaccion" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{0BAC5350-6187-4007-A1E7-9BB5CEF1C730}" name="frecuencia_de_pago" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{D476E092-13AF-42EE-AEEF-4CD702AD1094}" name="fecha_de_inicio" dataDxfId="31"/>
     <tableColumn id="4" xr3:uid="{6ABE0833-0B41-40A0-BBD8-C4A709289E9F}" name="cantidad_de_frecuencias"/>
     <tableColumn id="5" xr3:uid="{6575A171-3761-4E26-A921-5D5E48E4DE51}" name="dias_de_margen"/>
-    <tableColumn id="6" xr3:uid="{F9B5451D-FA90-48DF-80E4-7A84FC8C97DC}" name="monto_por_evento"/>
+    <tableColumn id="6" xr3:uid="{F9B5451D-FA90-48DF-80E4-7A84FC8C97DC}" name="monto_por_evento" dataDxfId="30"/>
     <tableColumn id="7" xr3:uid="{AC6E4DF5-AB72-4C52-A496-624BC2388908}" name="forma_de_pago" dataDxfId="29"/>
     <tableColumn id="8" xr3:uid="{678DB44A-A74D-4876-B5D1-F88C68C3EDAF}" name="descripcion" dataDxfId="28"/>
     <tableColumn id="9" xr3:uid="{681E92D6-501A-4714-B16D-3171F9FED5FD}" name="categoria" dataDxfId="27"/>
@@ -675,16 +677,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D79B7718-C5F9-44F4-99B0-95EC35A89BD8}" name="estructura_transacciones39" displayName="estructura_transacciones39" ref="A1:I3" totalsRowShown="0">
-  <autoFilter ref="A1:I3" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D79B7718-C5F9-44F4-99B0-95EC35A89BD8}" name="estructura_transacciones39" displayName="estructura_transacciones39" ref="A1:H3" totalsRowShown="0">
+  <autoFilter ref="A1:H3" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D240ED92-CE4A-4A49-B340-81EF262976A6}" name="fecha_de_cargo" dataDxfId="24"/>
     <tableColumn id="8" xr3:uid="{92A8E1F3-5EAF-4920-A91A-67C16A5C9192}" name="descripcion" dataDxfId="23"/>
     <tableColumn id="9" xr3:uid="{D9377D95-3CBB-4EFF-9FC3-1AE27C942399}" name="categoria" dataDxfId="22"/>
     <tableColumn id="6" xr3:uid="{6364E12B-6F00-4608-92D1-5AC72DA21B6C}" name="monto"/>
     <tableColumn id="7" xr3:uid="{15AB5548-E45C-4853-B770-F26EDF365AA3}" name="forma_de_pago" dataDxfId="21"/>
     <tableColumn id="10" xr3:uid="{3537C902-E7DB-47CB-B546-6A67D806A969}" name="realizado_por" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{A66D34F0-156E-421A-8D72-1285A90E997D}" name="limite_de_pago"/>
     <tableColumn id="5" xr3:uid="{1741BE5E-1D74-4650-BCB7-8823DCCFD4A0}" name="deuda_a_plazos_recurrente_o_normal"/>
     <tableColumn id="11" xr3:uid="{6EB0FDC1-CD9D-4F49-A0F1-F601EADB2F80}" name="comentarios" dataDxfId="19"/>
   </tableColumns>
@@ -1094,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214FC33E-AB93-4FE3-A38C-763F676E51D1}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1152,249 +1153,48 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45410</v>
+        <v>45228</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>45410</v>
+        <v>45228</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>12000</v>
+        <v>10000</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>45412</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45412</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>120000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>45416</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45417</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>146</v>
-      </c>
-      <c r="G4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>45416</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="1">
-        <v>45426</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5000</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>45416</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45426</v>
-      </c>
-      <c r="D6">
-        <v>24</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>10000</v>
-      </c>
-      <c r="G6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>45416</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45426</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>13000</v>
-      </c>
-      <c r="G7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>45416</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>45426</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>13000</v>
-      </c>
-      <c r="G8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{B21D9B68-801E-4EC4-81E1-F4276CBCE9B4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7E34192A-9AB8-42FB-A10E-6192E75DBF01}">
       <formula1>frecuencias_de_pago</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G8" xr:uid="{0E6FF20C-CD02-4622-8CE1-1AB3F846A768}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{4192880D-0BF5-436A-8A34-203481F6B560}">
       <formula1>creditos</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I8" xr:uid="{C19FE2FE-DD95-4099-B3F1-CAB3A01AE307}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{07C91FC5-FDCE-4BF9-B4AE-2F3AE6AA22DE}">
       <formula1>gastos_categories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J8" xr:uid="{9F71D4B4-97FF-4553-AE80-9F4138ED83CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{54069142-CEB2-424C-A129-B663BF0D7FC0}">
       <formula1>issued_by</formula1>
     </dataValidation>
   </dataValidations>
@@ -1407,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C2B398-A257-40E8-BC27-68B108BFDE7D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1418,35 +1218,29 @@
     <col min="1" max="1" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1454,51 +1248,39 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>19</v>
       </c>
       <c r="C4">
-        <v>19</v>
-      </c>
-      <c r="D4">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
       <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>26</v>
-      </c>
-      <c r="D6">
         <v>19</v>
       </c>
     </row>
@@ -1511,6 +1293,82 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85A8DC8-AF5B-4F72-9355-2F4A2A41DE09}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A1:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0811939C-0E2B-4C1B-A938-B33FF617EAE1}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -1522,12 +1380,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
@@ -1537,22 +1395,22 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1563,12 +1421,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595A5F2B-9BAB-4628-8C41-BD18B359C3F0}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1578,32 +1436,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1614,12 +1472,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2AA961-0E7B-4DEB-B9DA-A369758C8FB5}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="A10" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1629,22 +1487,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
@@ -1654,22 +1512,27 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1680,7 +1543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EC088D-A31B-40F5-B470-400E75CC1FF7}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -1693,22 +1556,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1721,11 +1584,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215E03AC-E0F3-4BB7-B8F8-865BC1096EBE}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1779,68 +1640,108 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45410</v>
+        <v>45556</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1">
-        <v>45410</v>
+        <v>45556</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>100</v>
+      <c r="F2" s="2">
+        <v>800</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>45433</v>
+      </c>
       <c r="B3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45433</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1800</v>
+      </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>106</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
-      </c>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>45433</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45433</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1800</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{51237FD8-298F-4C0B-B809-DC77A5FCEEAD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{E1A01DDE-ADE5-4AB2-A00A-E9B34637D814}">
       <formula1>frecuencias_de_pago</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{1A513A81-FF03-4AD3-AB6C-00DB494732EE}">
-      <formula1>payment_method</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{88F1C794-5AAE-4986-8B3C-4CF41D0B216B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{35840D09-514F-4340-87A4-EE6B2ECF3A24}">
       <formula1>issued_by</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3" xr:uid="{338B2AF6-838E-4EAB-BA1F-71E771CB8B0D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{262668A4-F67E-4A82-9BAA-E4FBE91BA7C6}">
       <formula1>gastos_categories</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{A5EDBBFD-BDB0-459C-A05E-BA859C3354A5}">
+      <formula1>payment_methods</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1852,26 +1753,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197764B1-063C-4E4D-BF12-01F672FAF6B9}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.90625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1894,63 +1796,70 @@
         <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45410</v>
+        <v>45422</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>45421</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
       </c>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{AD92261C-1E50-49C4-97FC-87A89E387766}">
-      <formula1>creditos</formula1>
+      <formula1>payment_methods</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{48CF1E6D-1F5E-4F41-9B93-3B6C39C02A8B}">
       <formula1>issued_by</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{468FA91C-F12A-4B09-8345-47EFF0D10FF8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{468FA91C-F12A-4B09-8345-47EFF0D10FF8}">
       <formula1>plazos_recurrente_normal</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{DE86E149-6802-4D3E-B8DE-9585938348B3}">
@@ -1969,7 +1878,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2117,13 +2026,13 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -2135,7 +2044,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1"/>
       <c r="I3" t="s">
@@ -2169,7 +2078,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2224,7 +2133,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -2239,7 +2148,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -2276,258 +2185,258 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2553,22 +2462,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2594,7 +2503,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -2604,32 +2513,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress from text to stg
</commit_message>
<xml_diff>
--- a/david_finance.xlsx
+++ b/david_finance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\python_codes\finance_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FFA578-7254-45C1-B5FD-7940E07B0904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874349C6-2C61-4733-9A67-9573CD4C11CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{345403B4-E0C2-451B-BA1E-8F2416887F82}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{345403B4-E0C2-451B-BA1E-8F2416887F82}"/>
   </bookViews>
   <sheets>
     <sheet name="deudas_a_plazos" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <definedName name="gastos_categories">gastos_categories!$A$2:$A$32</definedName>
     <definedName name="ingresos_categories">ingresos_categories!$A$2:$A$4</definedName>
     <definedName name="issued_by">issued_by!$A$2:$A$8</definedName>
-    <definedName name="payment_methods">payment_methods!$A$2:$A$11</definedName>
+    <definedName name="payment_methods">payment_methods!$A$2:$A$12</definedName>
     <definedName name="plazos_recurrente_normal">plazos_recurrente_normal!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4226" uniqueCount="147">
   <si>
     <t>fecha_de_transaccion</t>
   </si>
@@ -520,6 +520,18 @@
   <si>
     <t>Youtube Premium</t>
   </si>
+  <si>
+    <t>C&amp;A</t>
+  </si>
+  <si>
+    <t>Heb despensa</t>
+  </si>
+  <si>
+    <t>comercio</t>
+  </si>
+  <si>
+    <t>Heb</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -565,12 +577,11 @@
     <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="57">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -663,6 +674,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -3332,20 +3346,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}" name="estructura_transacciones" displayName="estructura_transacciones" ref="A1:K4" totalsRowShown="0">
-  <autoFilter ref="A1:K4" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3751A530-512A-48D0-ACA1-E2237E85BD4B}" name="fecha_de_transaccion" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{7385DBD7-EB34-433E-A7DB-728EAF33D62E}" name="frecuencia_de_pago" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{626C2B8F-5C27-4C0B-B719-5B93327D2501}" name="fecha_de_inicio" dataDxfId="53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}" name="estructura_transacciones" displayName="estructura_transacciones" ref="A1:L5" totalsRowShown="0">
+  <autoFilter ref="A1:L5" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{3751A530-512A-48D0-ACA1-E2237E85BD4B}" name="fecha_de_transaccion" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{7385DBD7-EB34-433E-A7DB-728EAF33D62E}" name="frecuencia_de_pago" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{626C2B8F-5C27-4C0B-B719-5B93327D2501}" name="fecha_de_inicio" dataDxfId="54"/>
     <tableColumn id="4" xr3:uid="{6FA13EEF-3757-406D-AB04-AE84D502C26F}" name="numero_de_plazos"/>
     <tableColumn id="5" xr3:uid="{69EFA34A-90CC-44D8-94DA-C15E94B31796}" name="dias_de_margen"/>
-    <tableColumn id="6" xr3:uid="{6FA1131D-FE42-43C8-9D6A-591D0F28EC2F}" name="monto_total_deuda" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{FD79B06C-466E-4B3B-92B7-9CC99AB235E6}" name="forma_de_pago" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{3B2495AD-A8F6-48EB-BEEF-5C6D9FDC70A4}" name="descripcion" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{6A11E9C5-3541-40DF-A991-FB22ABA03550}" name="categoria" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{E0E77362-FF5F-42CB-91DD-D5389F8891C5}" name="realizado_por" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{E46B6D76-C8A7-4B91-8651-7A3D1A573011}" name="comentarios" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{6FA1131D-FE42-43C8-9D6A-591D0F28EC2F}" name="monto_total_deuda" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{FD79B06C-466E-4B3B-92B7-9CC99AB235E6}" name="forma_de_pago" dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{8FB8CD14-5ED2-4AFE-B86C-B6C2B306BE59}" name="comercio"/>
+    <tableColumn id="8" xr3:uid="{3B2495AD-A8F6-48EB-BEEF-5C6D9FDC70A4}" name="descripcion" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{6A11E9C5-3541-40DF-A991-FB22ABA03550}" name="categoria" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{E0E77362-FF5F-42CB-91DD-D5389F8891C5}" name="realizado_por" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{E46B6D76-C8A7-4B91-8651-7A3D1A573011}" name="comentarios" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3414,7 +3429,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FB2F1B61-6BB5-4631-AA80-6C4EAC37AA8F}" name="tbl_payment_methods" displayName="tbl_payment_methods" ref="A1:A11" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FB2F1B61-6BB5-4631-AA80-6C4EAC37AA8F}" name="tbl_payment_methods" displayName="tbl_payment_methods" ref="A1:A12" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{3259DA84-A256-4980-9405-0F87438BFD13}" name="payment_methods"/>
   </tableColumns>
@@ -3464,13 +3479,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9EE98860-EFB6-4496-9DF4-B62DF57C1B3C}" name="deudas_a_plazos_detalle" displayName="deudas_a_plazos_detalle" ref="A1:I73" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I73" xr:uid="{9EE98860-EFB6-4496-9DF4-B62DF57C1B3C}"/>
   <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{676BB9E6-D690-4CA7-BB79-A522F271609F}" uniqueName="2" name="fecha_de_cargo" queryTableFieldId="2" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{676BB9E6-D690-4CA7-BB79-A522F271609F}" uniqueName="2" name="fecha_de_cargo" queryTableFieldId="2" dataDxfId="47"/>
     <tableColumn id="3" xr3:uid="{45E8B0BE-C03C-47E2-B133-B20E6E6FEDB9}" uniqueName="3" name="descripcion" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{81CF428F-FF73-47EC-AE77-5C8DDED45B4C}" uniqueName="4" name="categoria" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{68B3445F-73D2-4D9D-93E8-75F04C2B1AFB}" uniqueName="5" name="monto" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{FD602749-69E9-495C-AC91-E87365AE0D42}" uniqueName="6" name="forma_de_pago" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{B0F98B73-1C12-4FE9-B998-30AD246232AE}" uniqueName="7" name="realizado_por" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{429ED260-5282-4B52-A92A-A1514D46D415}" uniqueName="8" name="limite_de_pago" queryTableFieldId="8" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{429ED260-5282-4B52-A92A-A1514D46D415}" uniqueName="8" name="limite_de_pago" queryTableFieldId="8" dataDxfId="46"/>
     <tableColumn id="9" xr3:uid="{25F21882-83E1-407E-9375-E960BB44BAB9}" uniqueName="9" name="deuda_a_plazos_recurrente_o_normal" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{349FA1E1-7C3F-4E03-8FB1-09320A2ED911}" uniqueName="10" name="comentarios" queryTableFieldId="10"/>
   </tableColumns>
@@ -3479,20 +3494,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F622556F-D87B-4F08-9DB0-55027FD6196C}" name="estructura_transacciones3" displayName="estructura_transacciones3" ref="A1:K15" totalsRowShown="0">
-  <autoFilter ref="A1:K15" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{596EC6A4-11EF-4DEE-B34E-9EC3BA15F511}" name="fecha_de_transaccion" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{0BAC5350-6187-4007-A1E7-9BB5CEF1C730}" name="frecuencia_de_pago" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{D476E092-13AF-42EE-AEEF-4CD702AD1094}" name="fecha_de_inicio" dataDxfId="42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F622556F-D87B-4F08-9DB0-55027FD6196C}" name="estructura_transacciones3" displayName="estructura_transacciones3" ref="A1:L16" totalsRowShown="0">
+  <autoFilter ref="A1:L16" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{596EC6A4-11EF-4DEE-B34E-9EC3BA15F511}" name="fecha_de_transaccion" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{0BAC5350-6187-4007-A1E7-9BB5CEF1C730}" name="frecuencia_de_pago" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{D476E092-13AF-42EE-AEEF-4CD702AD1094}" name="fecha_de_inicio" dataDxfId="43"/>
     <tableColumn id="4" xr3:uid="{6ABE0833-0B41-40A0-BBD8-C4A709289E9F}" name="cantidad_de_frecuencias"/>
     <tableColumn id="5" xr3:uid="{6575A171-3761-4E26-A921-5D5E48E4DE51}" name="dias_de_margen"/>
-    <tableColumn id="6" xr3:uid="{F9B5451D-FA90-48DF-80E4-7A84FC8C97DC}" name="monto_por_evento" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{AC6E4DF5-AB72-4C52-A496-624BC2388908}" name="forma_de_pago" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{678DB44A-A74D-4876-B5D1-F88C68C3EDAF}" name="descripcion" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{681E92D6-501A-4714-B16D-3171F9FED5FD}" name="categoria" dataDxfId="38"/>
-    <tableColumn id="10" xr3:uid="{E2A3ADCC-528F-4870-AC9B-81F1C834529B}" name="realizado_por" dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{86797A6C-B13C-423C-AA63-09FCD4C63B28}" name="comentarios" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{F9B5451D-FA90-48DF-80E4-7A84FC8C97DC}" name="monto_por_evento" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{AC6E4DF5-AB72-4C52-A496-624BC2388908}" name="forma_de_pago" dataDxfId="41"/>
+    <tableColumn id="12" xr3:uid="{DA10E7CB-3C5C-42BC-8A2E-0FB436E4BD5B}" name="comercio"/>
+    <tableColumn id="8" xr3:uid="{678DB44A-A74D-4876-B5D1-F88C68C3EDAF}" name="descripcion" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{681E92D6-501A-4714-B16D-3171F9FED5FD}" name="categoria" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{E2A3ADCC-528F-4870-AC9B-81F1C834529B}" name="realizado_por" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{86797A6C-B13C-423C-AA63-09FCD4C63B28}" name="comentarios" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3502,13 +3518,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{10B198E7-78FB-40FD-9CF7-AF9A5F6109B6}" name="recurrentes_detalle" displayName="recurrentes_detalle" ref="A1:I233" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I233" xr:uid="{10B198E7-78FB-40FD-9CF7-AF9A5F6109B6}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{29EDD6D6-9D36-44B1-B542-3AA0E4064B24}" uniqueName="1" name="fecha_de_cargo" queryTableFieldId="1" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{29EDD6D6-9D36-44B1-B542-3AA0E4064B24}" uniqueName="1" name="fecha_de_cargo" queryTableFieldId="1" dataDxfId="36"/>
     <tableColumn id="2" xr3:uid="{C0738BE7-AC7E-4237-9472-B9E065110FF4}" uniqueName="2" name="descripcion" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{317F636F-7D4F-4342-81D9-63C9077FC09E}" uniqueName="3" name="categoria" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{EEF87649-FA29-4ABB-9AE2-1937F11DCBCE}" uniqueName="4" name="monto" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{0EDAE748-EFF2-4415-B783-2B5CEF2B78A4}" uniqueName="5" name="forma_de_pago" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{726C8122-6CD0-404E-B37D-F28BC0614DFF}" uniqueName="6" name="realizado_por" queryTableFieldId="6"/>
-    <tableColumn id="7" xr3:uid="{C69E7D5D-37B1-42C9-B648-BAE387734075}" uniqueName="7" name="limite_de_pago" queryTableFieldId="7" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{C69E7D5D-37B1-42C9-B648-BAE387734075}" uniqueName="7" name="limite_de_pago" queryTableFieldId="7" dataDxfId="35"/>
     <tableColumn id="8" xr3:uid="{6E4AD1D6-8840-420F-974B-1D8FEB1AF80A}" uniqueName="8" name="deuda_a_plazos_recurrente_o_normal" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{292FBE0B-CA6A-4859-A829-19F4CFD11F78}" uniqueName="9" name="comentarios" queryTableFieldId="9"/>
   </tableColumns>
@@ -3517,10 +3533,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D79B7718-C5F9-44F4-99B0-95EC35A89BD8}" name="estructura_transacciones39" displayName="estructura_transacciones39" ref="A1:G3" totalsRowShown="0">
-  <autoFilter ref="A1:G3" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D240ED92-CE4A-4A49-B340-81EF262976A6}" name="fecha_de_cargo" dataDxfId="33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D79B7718-C5F9-44F4-99B0-95EC35A89BD8}" name="estructura_transacciones39" displayName="estructura_transacciones39" ref="A1:H3" totalsRowShown="0">
+  <autoFilter ref="A1:H3" xr:uid="{6F05683C-0EAF-45BA-8056-546567C31854}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D240ED92-CE4A-4A49-B340-81EF262976A6}" name="fecha_de_cargo" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{C769C1A2-DAF1-4A46-BB66-3AA9BB4093E4}" name="comercio" dataDxfId="33"/>
     <tableColumn id="8" xr3:uid="{92A8E1F3-5EAF-4920-A91A-67C16A5C9192}" name="descripcion" dataDxfId="32"/>
     <tableColumn id="9" xr3:uid="{D9377D95-3CBB-4EFF-9FC3-1AE27C942399}" name="categoria" dataDxfId="31"/>
     <tableColumn id="6" xr3:uid="{6364E12B-6F00-4608-92D1-5AC72DA21B6C}" name="monto"/>
@@ -3926,10 +3943,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3941,13 +3958,14 @@
     <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3970,19 +3988,22 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>45383</v>
       </c>
@@ -4005,16 +4026,19 @@
         <v>63</v>
       </c>
       <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
         <v>107</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>40</v>
       </c>
-      <c r="J2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>45427</v>
       </c>
@@ -4036,17 +4060,17 @@
       <c r="G3" t="s">
         <v>94</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>113</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>45564</v>
       </c>
@@ -4068,34 +4092,52 @@
       <c r="G4" t="s">
         <v>65</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>136</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" t="s">
-        <v>68</v>
-      </c>
       <c r="K4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6">
+        <v>45570</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F8" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{7E34192A-9AB8-42FB-A10E-6192E75DBF01}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{7E34192A-9AB8-42FB-A10E-6192E75DBF01}">
       <formula1>frecuencias_de_pago</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{4192880D-0BF5-436A-8A34-203481F6B560}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H5" xr:uid="{4192880D-0BF5-436A-8A34-203481F6B560}">
       <formula1>creditos</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{07C91FC5-FDCE-4BF9-B4AE-2F3AE6AA22DE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{07C91FC5-FDCE-4BF9-B4AE-2F3AE6AA22DE}">
       <formula1>gastos_categories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{54069142-CEB2-424C-A129-B663BF0D7FC0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5" xr:uid="{54069142-CEB2-424C-A129-B663BF0D7FC0}">
       <formula1>issued_by</formula1>
     </dataValidation>
   </dataValidations>
@@ -5913,10 +5955,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5977,6 +6019,11 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -8361,10 +8408,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8376,13 +8423,14 @@
     <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8405,19 +8453,22 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>45425</v>
       </c>
@@ -8439,17 +8490,17 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>114</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>45438</v>
       </c>
@@ -8471,17 +8522,17 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>115</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>60</v>
       </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>45432</v>
       </c>
@@ -8503,17 +8554,17 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>116</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>60</v>
       </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>45429</v>
       </c>
@@ -8535,17 +8586,17 @@
       <c r="G5" t="s">
         <v>66</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>117</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>32</v>
       </c>
-      <c r="J5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>45383</v>
       </c>
@@ -8567,17 +8618,17 @@
       <c r="G6" t="s">
         <v>63</v>
       </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
       <c r="I6" t="s">
         <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>45383</v>
       </c>
@@ -8599,17 +8650,17 @@
       <c r="G7" t="s">
         <v>63</v>
       </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
       <c r="I7" t="s">
         <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>45412</v>
       </c>
@@ -8631,17 +8682,17 @@
       <c r="G8" t="s">
         <v>66</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>135</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>30</v>
       </c>
-      <c r="J8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>45412</v>
       </c>
@@ -8663,17 +8714,17 @@
       <c r="G9" t="s">
         <v>66</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>135</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>45473</v>
       </c>
@@ -8695,21 +8746,21 @@
       <c r="G10" t="s">
         <v>66</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>138</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>54</v>
       </c>
-      <c r="J10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>45417</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="6">
@@ -8724,25 +8775,24 @@
       <c r="F11" s="2">
         <v>129</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="I11" t="s">
         <v>139</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>45406</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="6">
@@ -8757,25 +8807,24 @@
       <c r="F12" s="2">
         <v>150</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="I12" t="s">
         <v>140</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>45406</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="6">
@@ -8790,25 +8839,24 @@
       <c r="F13" s="2">
         <v>169</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" t="s">
         <v>141</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="J13" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>45426</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="6">
@@ -8823,43 +8871,40 @@
       <c r="F14" s="2">
         <v>139</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I14" t="s">
         <v>142</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="J14" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
       <c r="C15" s="6"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C16" s="6"/>
+      <c r="F16" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{E1A01DDE-ADE5-4AB2-A00A-E9B34637D814}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16" xr:uid="{E1A01DDE-ADE5-4AB2-A00A-E9B34637D814}">
       <formula1>frecuencias_de_pago</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J15" xr:uid="{35840D09-514F-4340-87A4-EE6B2ECF3A24}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K16" xr:uid="{35840D09-514F-4340-87A4-EE6B2ECF3A24}">
       <formula1>issued_by</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I15" xr:uid="{262668A4-F67E-4A82-9BAA-E4FBE91BA7C6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J16" xr:uid="{262668A4-F67E-4A82-9BAA-E4FBE91BA7C6}">
       <formula1>gastos_categories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G15" xr:uid="{A5EDBBFD-BDB0-459C-A05E-BA859C3354A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H16" xr:uid="{A5EDBBFD-BDB0-459C-A05E-BA859C3354A5}">
       <formula1>payment_methods</formula1>
     </dataValidation>
   </dataValidations>
@@ -8877,7 +8922,9 @@
   </sheetPr>
   <dimension ref="A1:I233"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15662,101 +15709,107 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45422</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+        <v>45565</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>2585.35</v>
+      </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>45421</v>
+        <v>45565</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>604.39</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{AD92261C-1E50-49C4-97FC-87A89E387766}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{AD92261C-1E50-49C4-97FC-87A89E387766}">
       <formula1>payment_methods</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{48CF1E6D-1F5E-4F41-9B93-3B6C39C02A8B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{48CF1E6D-1F5E-4F41-9B93-3B6C39C02A8B}">
       <formula1>issued_by</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{DE86E149-6802-4D3E-B8DE-9585938348B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{DE86E149-6802-4D3E-B8DE-9585938348B3}">
       <formula1>gastos_categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -15774,8 +15827,8 @@
   </sheetPr>
   <dimension ref="A1:I307"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24712,7 +24765,7 @@
   <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>